<commit_message>
Edited cheatsheets and added HCI and Comp and Cloud
</commit_message>
<xml_diff>
--- a/Python, NumPy, Pandas, MatPlotLib, Scikit-learn.xlsx
+++ b/Python, NumPy, Pandas, MatPlotLib, Scikit-learn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F002A51-9437-45E0-98D2-471421FCDC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6668582-22DE-489A-971B-285ECE6B7CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="741" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="16335" windowHeight="15585" tabRatio="741" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Python Intermediate" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="13">
+  <futureMetadata name="XLRICHVALUE" count="14">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -128,8 +128,15 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="13">
+  <valueMetadata count="14">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -169,12 +176,15 @@
     <bk>
       <rc t="1" v="12"/>
     </bk>
+    <bk>
+      <rc t="1" v="13"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="330">
   <si>
     <t>What we're doing</t>
   </si>
@@ -708,9 +718,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>1. Implement a recursive function to compute the nth Fibonacci number. The function should accept 3 arguments, two of them should have default values. The recursion begins with a single argument</t>
-  </si>
-  <si>
     <t>def fib(n):
     a, b = 0, 1
     for _ in range(n):
@@ -719,21 +726,8 @@
 fib(8)</t>
   </si>
   <si>
-    <t>2. Using a lambda, use filter() to accept a list and filter the integers that are divisible by 3. Use the modulus operator.</t>
-  </si>
-  <si>
-    <t>list1 = [3, 4, 7, 8, 9, 12, 13]
-list(filter(lambda x : x % 3 == 0, list1))</t>
-  </si>
-  <si>
-    <t>3. Using a lambda, use filter() to accept a list of pairs and accept the pairs whose elements are equal.</t>
-  </si>
-  <si>
     <t>list2 = [[1,1], [2, 5], [4, 4], [9, 9], [5, 3]]
 x = list(filter(lambda x : x[0] == x[1], list2))</t>
-  </si>
-  <si>
-    <t>4. Using a lambda, implement a map() that accepts a list of lists and returns the sums of the sublists</t>
   </si>
   <si>
     <t>list3 = [[1, 5, 3], [3, 6], [9, 11, 45, 11], [5, 2, 6, 3, 7]]
@@ -744,51 +738,12 @@
 print(emptyList)</t>
   </si>
   <si>
-    <t>5. Use the reduce() function to implement factorial, N!.</t>
-  </si>
-  <si>
-    <t>from functools import reduce
-reduce(lambda x, y: x+y, list(range(1,11)))</t>
-  </si>
-  <si>
-    <t>6. Write a function, called Convolve, that accepts three arguments. The first argument is a function. The second and third arguments will be used as arguments for the first argument, the function, by Convolve. Convolve will return the results packaged in a list. For example:</t>
-  </si>
-  <si>
     <t>def convolve(mapFunction, function1, list1):
     return list(mapFunction(function1, list1))
 convolve(map, lambda x : sum(x), list3)</t>
   </si>
   <si>
-    <t>Explanation:
-- The filter function is used to filter elements from list1 based on a condition.
-- The condition is defined using a lambda function: lambda x: x % 3 == 0. This lambda function takes a value x and returns True if x is divisible by 3, and False otherwise.
-- The filter function is applied to each element in list1. Only the elements for which the lambda function returns True are included in the result.
-- In this case, it filters out elements in list1 that are not divisible by 3.
-- The result is then converted to a list using list() and stored in the variable result.
-- So, after running this code, the result variable will contain a list of elements from list1 that are divisible by 3. In this example, the result would be [3, 9, 12].</t>
-  </si>
-  <si>
-    <t>This code filters pairs in list2 where the first and second elements are equal, creating a list x with those pairs. The lambda function checks if the first element (x[0]) is equal to the second element (x[1]).</t>
-  </si>
-  <si>
     <t>This code calculates the sum of each sublist in list3 using a lambda function (result1). The sums are then appended to a new list (emptyList), and the final result is printed.</t>
-  </si>
-  <si>
-    <t>This code defines a function named convolve that takes three parameters:
-1. mapFunction: A function that applies another function to elements of a list.
-2. function1: The function to be applied to the elements of the list.
-3. list1: The list of elements to which function1 is applied.
-- The convolve function uses mapFunction to apply function1 to each element of list1, and the result is returned as a list.
-- The provided example calls convolve with map as the mapFunction, a lambda function lambda x: sum(x) as function1, and list3 as list1. It essentially applies the sum function to each sublist in list3 using map, producing a list of the sums</t>
-  </si>
-  <si>
-    <t>Here's how the lambda function with two arguments (x and y) is used within the reduce function:
-list(range(1, 11)):  This generates a list containing the numbers from 1 to 10.
-reduce(lambda x, y: x + y, ...):  The reduce function takes two arguments: the binary function (lambda function) and an iterable.
-The lambda function, lambda x, y: x + y, specifies how to combine two elements at a time.
-The iterable is the list generated by list(range(1, 11)).
-So, during each iteration of reduce, the lambda function is applied to pairs of elements from the list. The x and y in the lambda function represent these two elements at each step of the iteration. The result of each operation becomes the new x for the next iteration, and the next element in the list becomes y. This process continues until the entire list is reduced to a single result, which is the sum of all the numbers from 1 to 10
-TLDR: when we do reduce with a list, because it does iteration, x and y automatically refer to list[0] and list[1], add them together, and then move onto the next value. It's very confusing, but it just means that we are able to loop through the list. This is kind of confusing</t>
   </si>
   <si>
     <t>Property decorator for Python methods</t>
@@ -2612,6 +2567,165 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">List of most useful methods and what they do:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n_samples = 150</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Creates 150 pieces of data
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n_features = 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Makes the data three dimensional (e.g. the data would be: ([3, 4, 5], [5, 6, 1], [9, 0, 1]… etc))
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>centers = 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - The number of clusters of data to generate
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cluster_std = 0.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - How spread out the data is. The closer to 0, the more compressed the data points, the closer to 1 the more spread
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shuffle = True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Shuffles the data once it has already been generated. It doesn't affect the data if/when it's plotted: it just randomises the order in which data appears in the dataset
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>random_state = 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Generates the same random data every time. Used for reproductability
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>center_box = (-10, 10)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Makes the range of the data between -10 to 10</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">List of the most useful parameters for Kmeans and what they do:
 </t>
     </r>
@@ -2699,7 +2813,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - The number of times the operation will be run with different centroid seeds
+      <t xml:space="preserve"> - The number of times the operation will be run with different centroid seeds. It actually grabs the best of the 10 iterations, and does the max_iterations over this best one
 </t>
     </r>
     <r>
@@ -2768,8 +2882,97 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">List of most useful methods and what they do:
+    <t>Cleaning data</t>
+  </si>
+  <si>
+    <t>One of the most important things that we do within AI is we have to handle, filter, and clean the data. This can be done through a combination of removing columns which have too many empty data sets, and filling in columns which have some empty data sets, perhaps by filling the blank spaces (.filna) with .mean() if the columns have numerical data. Also could possibly drop individual sets of data if they're outliers in the data.</t>
+  </si>
+  <si>
+    <t>Create encoded data using the Scikit-learn OneHotEncoder</t>
+  </si>
+  <si>
+    <t>OneHotEncoder Features expanded</t>
+  </si>
+  <si>
+    <r>
+      <t>.categories</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Shows the different category names </t>
+    </r>
+  </si>
+  <si>
+    <t>OneHotEncoder after the processing</t>
+  </si>
+  <si>
+    <r>
+      <t>df["Female"] = values[:, 0]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Creates new DataFrame column called females and assigns individuals who were female to have the value 1 in this column</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+df["Male"] = values[:, 1]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Same thing but for males</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+df.drop(columns=["Sex"])</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Drop the "Sex" column</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Import OneHotEncoder into the program
 </t>
     </r>
     <r>
@@ -2781,7 +2984,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>n_samples = 150</t>
+      <t>from sklearn.preprocessing import OneHotEncoder</t>
     </r>
     <r>
       <rPr>
@@ -2791,7 +2994,8 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - Creates 150 pieces of data
+      <t xml:space="preserve">
+# Create an instance of OneHotEncoder
 </t>
     </r>
     <r>
@@ -2803,7 +3007,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>n_features = 3</t>
+      <t>encoder = OneHotEncoder()</t>
     </r>
     <r>
       <rPr>
@@ -2813,7 +3017,8 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - Makes the data three dimensional (e.g. the data would be: ([3, 4, 5], [5, 6, 1], [9, 0, 1]… etc))
+      <t xml:space="preserve">
+# Fit and transform your categorical data
 </t>
     </r>
     <r>
@@ -2825,7 +3030,449 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>centers = 3</t>
+      <t>values = encoder.fit_transform(categorical_data)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>enc.categories_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Print out the categories of values</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We first of all import </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">OneHotEncoder </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sklearn.preprocessing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Next, we have to create the encoder by creating an encoder object with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OneHotEncoder().</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> There are a number of parameters we can pass through, but the primary ones will be </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>handle_unknown="ignore"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">sparce="false" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(returns data in a dense array format, to allow for all stored elements in the data). Finally, we can produced the encoded data using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>encoder.fit_transform([dataset])</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. The encoded data can be saved to a variable, let's say values, and within it will contain all the different types of the column (e.g. it will have "male" and "female" for each of the data points). After this you can add this data to your columns individually. One of the other key things to know about is the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.categories_ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">attribute, which will print out all of the column types that you have, to help you fill up the DataFrame afterwards (e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>categories_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> might contain ["female", "male"], which means that when you go to insert new values in the columns, you need to know that the female label is [0] and the male label is [1].</t>
+    </r>
+  </si>
+  <si>
+    <t>OneHotEncoding isn't used at the final step. It's more just a tool to help you before the data is processed, so it's a tool that is then used in other machine learning algorithms/models.</t>
+  </si>
+  <si>
+    <t>Implement a recursive function to compute the nth Fibonacci number. The function should accept 3 arguments, two of them should have default values. The recursion begins with a single argument</t>
+  </si>
+  <si>
+    <t>Using a lambda, use filter() to accept a list and filter the integers that are divisible by 3. Use the modulus operator.</t>
+  </si>
+  <si>
+    <t>Using a lambda, use filter() to accept a list of pairs and accept the pairs whose elements are equal.</t>
+  </si>
+  <si>
+    <t>Using a lambda, implement a map() that accepts a list of lists and returns the sums of the sublists</t>
+  </si>
+  <si>
+    <t>Use the reduce() function to implement factorial, N!.</t>
+  </si>
+  <si>
+    <t>Write a function, called Convolve, that accepts three arguments. The first argument is a function. The second and third arguments will be used as arguments for the first argument, the function, by Convolve. Convolve will return the results packaged in a list. For example:</t>
+  </si>
+  <si>
+    <t>Simple lambda</t>
+  </si>
+  <si>
+    <t>z = lambda x: x ** 2
+print(z(8))
+# Will print 64</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The order of lambda used in this simple way is:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">lambda aurguments: expression
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">In the example to the left, we are passing through 8 as our argument, and we are ouputting 64. The expression, once it's been calcluated, looks like: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lambda 8 : 8**2</t>
+    </r>
+  </si>
+  <si>
+    <t>list1 = [3, 4, 7, 8, 9, 12, 13]
+output = list(filter(lambda x : x % 3 == 0, list1))
+print(output)
+# Will print out [2, 4, 6, 8]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The code filters elements from list1 that are divisible by 3. Here's a simplified breakdown:
+1. A lambda function checks if a number is divisible by 3: lambda x: x % 3 == 0.
+2. The filter() function applies this lambda function to each element in list1.
+3. Only elements for which the lambda function returns True (i.e., those divisible by 3) are included.
+4. The filtered elements are converted to a list and stored in the variable result.
+5. After running the code, result will contain a list of elements from list1 that are divisible by 3, e.g., [3, 9, 12].
+The structure of the entire statement is like this:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">list(filter(lambda argument: expression, entire list)), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>where the list has the same name, and is in fact in direct reference to the actual list that we're bringing in.</t>
+    </r>
+  </si>
+  <si>
+    <t>from functools import reduce
+p = [1, 2, 3, 4, 5, 6, 7, 8, 9]
+print(reduce (lambda x, y: x + y, p))
+# prints 45</t>
+  </si>
+  <si>
+    <t>In the expression reduce(lambda x, y: x + y, list(range(1, 11))), the lambda function lambda x, y: x + y specifies how to combine two elements at a time. When reduce() is used with a list, it iterates through the list, and x and y automatically represent the first two elements in the list. The lambda function then adds them together. This process continues, with the result of each operation becoming the new x for the next iteration, and the next element in the list becoming y. This iteration continues until the entire list is reduced to a single result, which is the sum of all the numbers from 1 to 10.
+Reduce is used for cumulative frequencies. If we have a list with three values, then in the first round, x and y will actually represent the first and second value the first time. On the second round, x will represent the result of the previous round, and y will represent the third value.</t>
+  </si>
+  <si>
+    <t>This code filters pairs in list2 where the first and second elements are equal, creating a list x with those pairs. The lambda function checks if the first element (x[0]) is equal to the second element (x[1]).
+This is a similar example to the former list, but now that we're iterating through a list of lists, each x (each item we go through) now has multiple items within it. It basically checks if the expression is true, and if it is, then append it to the list. If not, then don't append it. This is the reason why if statements are used for filters.</t>
+  </si>
+  <si>
+    <t>This code defines a function called convolve that takes three parameters:
+- mapFunction: A function that applies another function to elements of a list.
+- function1: The function to be applied to the elements of the list.
+- list1: The list of elements to which function1 is applied.
+The convolve function utilizes mapFunction to apply function1 to each element of list1, and then returns the result as a list. In the provided example, convolve is invoked with map as the mapFunction, a lambda function lambda x: sum(x) as function1, and list3 as list1. Essentially, it applies the sum function to each sublist in list3 using map, resulting in a list of sums.
+Basically, it's like the filter function, but instead of checking for true or false, it just appends it to the list.</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There are two main stages: the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>classification algorithm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">classication model; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">the former helping to build the latter. There are multiple types of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>classification algorithms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that exist, which can be used for building a classification model. You could also have a situation where you build an initial </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>classification model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, it works normally, but then you get more training examples, and you may find it in your best interest to rebuild a new classification model.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A form of supervised learning, it consists of finding a model that is able to predict the value of a target (class) attribute of an example based on the values of a set of predictor attributes. E.g. for breast cancer, the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">predictor attributes </t>
     </r>
     <r>
       <rPr>
@@ -2835,95 +3482,452 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - The number of clusters of data to generate
+      <t xml:space="preserve">would be left/right breast, tumour size, age, and whether it's been irradiated or not, and the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>class attribute</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is the recurrence of breast cancer. This supervised learning relies on a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>training set</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (basically, relies on real world data that already exists. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Past data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) in order to predict the class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of a test set</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>future data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">from sklearn.tree import DecisionTreeClassifier
+# prepares the training data
 </t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cluster_std = 0.5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">X_train = iris_data.loc[:, 'sepal length':'petal width']
+y_train = iris_data['class']
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t># builds the classifier
+tree = DecisionTreeClassifier()
+tree.fit(X_train, y_train)
+# Test the items
+tree.score(X_train2, Y_train2)</t>
+    </r>
+  </si>
+  <si>
+    <t>Export the tree data as text, and show the DecisionTree data as a plot</t>
+  </si>
+  <si>
+    <t>from sklearn.tree import export_text
+from sklearn.tree import plot_tree
+# Export as text data
+text_representation = export_text(tree)
+print(text_representation)
+# graphic representation
+fig = plt.figure(figsize=(25,20))
+_ = plot_tree(tree, feature_names=columns, class_names=y_train.values, filled=True)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">One of the most common methods of working with predictor attributes (X_train) and class attributes (Y_train) is using the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DecisionTreeClassifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> module in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sklearn.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The predictor attributes must have all the data properly filtered (we've selected all the data using the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>colon :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), and include all the columns (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[first column]: [to the last column of the predictor attribute]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">). We then map this to the class attribute, which is only allowed to be one column of data. Afterwards, we build the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DecisionTreeClassifier()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, give it a name, and then fit the X_train and Y_train using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tree.fit(X_train, Y_train)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - How spread out the data is. The closer to 0, the more compressed the data points, the closer to 1 the more spread
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>shuffle = True</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t xml:space="preserve">
+Finally, when we use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tree.score(x, y)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> this produces a tree score, a number between 0 and 1 to see how accurate our model is: 0 being 100% wrong, 1 being 100% correct.</t>
+    </r>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>A form of supervised learning, it is similar to classification, but not quite the same. It consists of finding a model that maps a given input to a numeric prediction (e.g. like attempting to predict house prices using a bunch of categories such as location, number of rooms, size, etc). The class attributre is a continuous variable, and will provide you with a real number</t>
+  </si>
+  <si>
+    <t>Lineal model for regression</t>
+  </si>
+  <si>
+    <t># Import the module
+from sklearn import linear_model
+# Create the linear regression model
+regressor = linear_model.LinearRegression()
+regressor.fit(X_train, y_train)
+# shows the coefficients of the linear model
+regressor.coef_</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Using a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DecisionTreeClassifier</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We start by importing the module, before creating our regressor. Next, we </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - Shuffles the data once it has already been generated. It doesn't affect the data if/when it's plotted: it just randomises the order in which data appears in the dataset
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>random_state = 0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>fit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - Generates the same random data every time. Used for reproductability
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>center_box = (-10, 10)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t xml:space="preserve"> the data using our </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - Makes the range of the data between -10 to 10</t>
+      <t xml:space="preserve">X_train </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y_train</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> model. Finally, we can see the relative weights of each of the columns using the relative weights using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.coef_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
     </r>
   </si>
 </sst>
@@ -2931,12 +3935,33 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3057,6 +4082,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3145,32 +4179,59 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3179,61 +4240,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3242,10 +4276,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3255,6 +4310,35 @@
   <dxfs count="106">
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3280,35 +4364,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4049,7 +5104,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="13">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="14">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -4102,6 +5157,10 @@
     <v>12</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -4129,6 +5188,7 @@
   <rel r:id="rId11"/>
   <rel r:id="rId12"/>
   <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
 </richValueRels>
 </file>
 
@@ -4175,8 +5235,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{46C16BA2-61C0-4599-920E-0C9F452559FA}" name="Table210" displayName="Table210" ref="A1:D7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:D7" xr:uid="{46C16BA2-61C0-4599-920E-0C9F452559FA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{46C16BA2-61C0-4599-920E-0C9F452559FA}" name="Table210" displayName="Table210" ref="A1:D10" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:D10" xr:uid="{46C16BA2-61C0-4599-920E-0C9F452559FA}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{23F4172E-BA4C-4B53-8A90-E0059ED1DE4A}" name="Concepts" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{04ADC2BE-761C-4A23-BD42-73FBD7BB9ACC}" name="General Understanding" dataDxfId="11"/>
@@ -4188,22 +5248,22 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FAF65583-B8F6-40EA-862C-E4025F5D5778}" name="Table114" displayName="Table114" ref="A1:E8" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
-  <autoFilter ref="A1:E8" xr:uid="{FAF65583-B8F6-40EA-862C-E4025F5D5778}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FAF65583-B8F6-40EA-862C-E4025F5D5778}" name="Table114" displayName="Table114" ref="A1:E12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
+  <autoFilter ref="A1:E12" xr:uid="{FAF65583-B8F6-40EA-862C-E4025F5D5778}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9DCDC563-2DFF-40C4-9194-5C07503E012F}" name="What we're doing" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{D5AE45F1-A084-45BD-B4F4-32098DA0FE85}" name="Code" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B8842199-257D-476D-91B8-BF5565E0CEB6}" name="Explained" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A56794F9-07D7-460B-9613-488C3E6D3E08}" name="Notes" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{58712703-E0DE-497F-99CA-53F643C2130A}" name="Images" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9DCDC563-2DFF-40C4-9194-5C07503E012F}" name="What we're doing" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{D5AE45F1-A084-45BD-B4F4-32098DA0FE85}" name="Code" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B8842199-257D-476D-91B8-BF5565E0CEB6}" name="Explained" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A56794F9-07D7-460B-9613-488C3E6D3E08}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{58712703-E0DE-497F-99CA-53F643C2130A}" name="Images" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7FD86BF1-CE00-4BA1-8920-1708F0222CC4}" name="Table6" displayName="Table6" ref="A1:C8" totalsRowShown="0" headerRowDxfId="96">
-  <autoFilter ref="A1:C8" xr:uid="{7FD86BF1-CE00-4BA1-8920-1708F0222CC4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7FD86BF1-CE00-4BA1-8920-1708F0222CC4}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0" headerRowDxfId="96">
+  <autoFilter ref="A1:C9" xr:uid="{7FD86BF1-CE00-4BA1-8920-1708F0222CC4}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{19453ECD-E5C7-401A-B7FC-87A649435C5C}" name="Description" dataDxfId="95"/>
     <tableColumn id="2" xr3:uid="{1919C35A-308E-40D1-AAC4-2CB4DF436B7C}" name="Code" dataDxfId="94"/>
@@ -4572,8 +5632,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4614,7 +5674,7 @@
         <v>107</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45">
@@ -4628,12 +5688,12 @@
         <v>110</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="120">
       <c r="A4" s="1" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>111</v>
@@ -4642,7 +5702,7 @@
         <v>112</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="225">
@@ -4672,82 +5732,82 @@
     </row>
     <row r="7" spans="1:5" ht="165">
       <c r="A7" s="1" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="270">
       <c r="A8" s="1" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="180">
       <c r="A9" s="1" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="90">
       <c r="A10" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
       <c r="A11" s="1" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="180">
       <c r="A12" s="1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="210">
       <c r="A13" s="1" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -4797,13 +5857,13 @@
     </row>
     <row r="2" spans="1:5" ht="60">
       <c r="A2" s="19" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -4852,32 +5912,32 @@
     </row>
     <row r="2" spans="1:5" ht="105">
       <c r="A2" s="1" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="19" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="19" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4890,26 +5950,25 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87179907-4FD1-4D78-B59B-9D41D9D2BE6B}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="2" max="3" width="80.28515625" customWidth="1"/>
     <col min="4" max="4" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="24" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>3</v>
@@ -4918,9 +5977,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="110.25" customHeight="1">
+    <row r="2" spans="1:4">
       <c r="A2" s="24" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -4928,63 +5987,99 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="105">
+    <row r="3" spans="1:4" ht="60">
       <c r="A3" s="24" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
     </row>
-    <row r="4" spans="1:4" ht="165">
+    <row r="4" spans="1:4" ht="105">
       <c r="A4" s="24" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="D4" s="24" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="117.75" customHeight="1">
+    <row r="5" spans="1:4" ht="60">
       <c r="A5" s="24" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="240">
+    <row r="6" spans="1:4" ht="150">
       <c r="A6" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>284</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>296</v>
-      </c>
       <c r="D6" s="24"/>
     </row>
-    <row r="7" spans="1:4" ht="150">
+    <row r="7" spans="1:4" ht="105">
       <c r="A7" s="24" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>286</v>
-      </c>
-      <c r="C7" s="24"/>
+        <v>274</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>301</v>
+      </c>
       <c r="D7" s="24"/>
+    </row>
+    <row r="8" spans="1:4" ht="90">
+      <c r="A8" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:4" ht="105">
+      <c r="A9" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:4" ht="75">
+      <c r="A10" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4996,10 +6091,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B3B599-2C6A-4CA8-B2F0-63091B448B87}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5031,38 +6126,38 @@
     </row>
     <row r="2" spans="1:5" ht="60">
       <c r="A2" s="31" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="D2" s="31"/>
       <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:5" ht="195">
       <c r="A3" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>290</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>291</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>292</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>303</v>
       </c>
       <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" ht="360">
       <c r="A4" s="32" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5070,47 +6165,101 @@
     </row>
     <row r="5" spans="1:5" ht="240">
       <c r="A5" s="31" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>298</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>302</v>
+        <v>286</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>291</v>
       </c>
       <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:5" ht="405">
       <c r="A6" s="32" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
+    <row r="7" spans="1:5" ht="195">
+      <c r="A7" s="34" t="s">
+        <v>294</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>300</v>
+      </c>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
+    <row r="8" spans="1:5" ht="60">
+      <c r="A8" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>298</v>
+      </c>
+      <c r="C8" s="34"/>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="34" t="s">
+        <v>295</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+    </row>
+    <row r="10" spans="1:5" ht="180">
+      <c r="A10" s="39" t="s">
+        <v>328</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="1:5" ht="165">
+      <c r="A11" s="39" t="s">
+        <v>321</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>322</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+    </row>
+    <row r="12" spans="1:5" ht="135">
+      <c r="A12" s="39" t="s">
+        <v>326</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>327</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>329</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5123,17 +6272,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5801CF83-070A-43B8-8C37-B014B6412981}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="66.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="57.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="83.85546875" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -5150,83 +6299,95 @@
     </row>
     <row r="2" spans="1:3" ht="90">
       <c r="A2" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" ht="75">
+      <c r="A3" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="180">
+      <c r="A4" s="36" t="s">
+        <v>303</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>311</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="120">
+      <c r="A5" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="13"/>
-    </row>
-    <row r="3" spans="1:3" ht="150">
-      <c r="A3" s="14" t="s">
+      <c r="C5" s="16" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="90">
+      <c r="A6" s="36" t="s">
+        <v>305</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C6" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="180">
+      <c r="A7" s="37" t="s">
+        <v>306</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>313</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="180">
+      <c r="A8" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="45">
-      <c r="A4" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="90">
-      <c r="A5" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="285">
-      <c r="A6" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="135">
-      <c r="A7" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="165">
-      <c r="A8" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>236</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>237</v>
+      <c r="C8" s="17" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="165">
+      <c r="A9" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5307,13 +6468,13 @@
     </row>
     <row r="5" spans="1:5" ht="45">
       <c r="A5" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="1"/>
@@ -5333,16 +6494,16 @@
     </row>
     <row r="7" spans="1:5" ht="60">
       <c r="A7" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -5505,13 +6666,13 @@
     </row>
     <row r="19" spans="1:5" ht="135">
       <c r="A19" s="1" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -5563,79 +6724,79 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
       <c r="A4" s="1" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="105">
       <c r="A6" s="1" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60">
       <c r="A7" s="1" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="180">
       <c r="A8" s="1" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -5684,71 +6845,71 @@
     </row>
     <row r="2" spans="1:5" ht="45">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="1" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45">
       <c r="A4" s="1" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
       <c r="A5" s="1" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="A6" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="75">
       <c r="A7" s="1" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -5813,13 +6974,13 @@
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="19" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -5875,7 +7036,7 @@
         <v>70</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C8" s="9"/>
     </row>
@@ -5910,51 +7071,51 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="19" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="C12" s="19"/>
     </row>
     <row r="13" spans="1:5" ht="210">
       <c r="A13" s="22" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="165">
       <c r="A14" s="22" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="C14" s="22"/>
     </row>
     <row r="15" spans="1:5" ht="150">
       <c r="A15" s="22" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="C15" s="22"/>
     </row>
     <row r="16" spans="1:5" ht="30">
       <c r="A16" s="23" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -6036,82 +7197,82 @@
     </row>
     <row r="5" spans="1:5" ht="60">
       <c r="A5" s="1" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="75">
       <c r="A6" s="1" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
       <c r="A7" s="1" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45">
       <c r="A8" s="1" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="105">
       <c r="A9" s="1" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45">
       <c r="A10" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="75">
       <c r="A11" s="22" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -6160,23 +7321,23 @@
     </row>
     <row r="2" spans="1:5" ht="255">
       <c r="A2" s="1" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -6234,7 +7395,7 @@
         <v>87</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="135">
@@ -6242,7 +7403,7 @@
         <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>90</v>
@@ -6287,7 +7448,7 @@
         <v>97</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Updated Scikit-learn information to include RandomTreeClassifiers
</commit_message>
<xml_diff>
--- a/Python, NumPy, Pandas, MatPlotLib, Scikit-learn.xlsx
+++ b/Python, NumPy, Pandas, MatPlotLib, Scikit-learn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6668582-22DE-489A-971B-285ECE6B7CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1854FDF9-A803-4094-A131-A1726172B6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="16335" windowHeight="15585" tabRatio="741" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="5895" windowWidth="29040" windowHeight="15720" tabRatio="741" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Python Intermediate" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="14">
+  <futureMetadata name="XLRICHVALUE" count="15">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -135,8 +135,15 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="14"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="14">
+  <valueMetadata count="15">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -179,12 +186,15 @@
     <bk>
       <rc t="1" v="13"/>
     </bk>
+    <bk>
+      <rc t="1" v="14"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="340">
   <si>
     <t>What we're doing</t>
   </si>
@@ -2972,101 +2982,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve"># Import OneHotEncoder into the program
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>from sklearn.preprocessing import OneHotEncoder</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-# Create an instance of OneHotEncoder
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>encoder = OneHotEncoder()</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-# Fit and transform your categorical data
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>values = encoder.fit_transform(categorical_data)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>enc.categories_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Print out the categories of values</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">We first of all import </t>
     </r>
     <r>
@@ -3930,17 +3845,248 @@
       <t>.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Import OneHotEncoder into the program
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>from sklearn.preprocessing import OneHotEncoder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+# Create an instance of OneHotEncoder
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>encoder = OneHotEncoder()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+# Fit and transform your categorical data
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>values = encoder.fit_transform(categorical_data)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>enc.categories_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Print out the categories of values</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If you want to select specific items for x_training, you can write it in like this:
+X_train = iris_data.loc[:, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>["attribute1", "attribute2", "attribute4", "attribute5",… etc]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>Confusion matrix</t>
+  </si>
+  <si>
+    <t>Train and test partition</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">from sklearn.model_selection import train_test_split
+X = iris_data.loc[:, 'sepal length':'petal width']
+y = iris_data['class']
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+# splits the data in training + testing
+X_train, X_test, y_train, y_test = train_test_split(X, y, random_state=0)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t># builds the classifier
+tree = DecisionTreeClassifier()
+tree.fit(X_train, y_train)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+# evaluates on the test data
+tree.score(X_test, y_test)
+# displays the confusion matrix
+predictions = tree.predict(X_test)
+cm = confusion_matrix(y_test, predictions, labels=tree.classes_)
+disp = ConfusionMatrixDisplay(confusion_matrix=cm, display_labels=tree.classes_)
+_ = disp.plot()</t>
+    </r>
+  </si>
+  <si>
+    <t>from sklearn.metrics import confusion_matrix, ConfusionMatrixDisplay
+predictions = tree.predict(X_train)
+cm = confusion_matrix(y_train, predictions, labels=tree.classes_)
+disp = ConfusionMatrixDisplay(confusion_matrix=cm, display_labels=tree.classes_)
+# displays the matrix
+_ = disp.plot()</t>
+  </si>
+  <si>
+    <t>A confusion matrix is just a way to see where errors in the model have been made. You have a chart, in which you hope that the only section that is highlighted is the diagonal bit (because you hope that there aren't any outliers in the data).</t>
+  </si>
+  <si>
+    <t>We can train and test the partition that we build using this method. What we're doing we we're splitting the dataset into two sections: a portion for testing, and a portion for training. It gives a better indication of the quality of the model.</t>
+  </si>
+  <si>
+    <t>RandomForestClassifier</t>
+  </si>
+  <si>
+    <t>from sklearn.ensemble import RandomForestClassifier
+forest = RandomForestClassifier(n_estimators=10, random_state=0)
+forest.fit(x_train, y_train)
+forest.score(x_train, y_train)</t>
+  </si>
+  <si>
+    <t>A RandomForestClassifier does a similar thing to the DecisionTreeClassifier, but it actually uses multiple decision trees (uses 10 in the example specified). The RandomForestClassifier requires more processing, but is also generally speaking more accurate.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4179,59 +4325,71 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4240,34 +4398,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4276,31 +4422,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5104,7 +5256,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="14">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="15">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -5161,6 +5313,10 @@
     <v>13</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>14</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -5189,6 +5345,7 @@
   <rel r:id="rId12"/>
   <rel r:id="rId13"/>
   <rel r:id="rId14"/>
+  <rel r:id="rId15"/>
 </richValueRels>
 </file>
 
@@ -5248,8 +5405,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FAF65583-B8F6-40EA-862C-E4025F5D5778}" name="Table114" displayName="Table114" ref="A1:E12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
-  <autoFilter ref="A1:E12" xr:uid="{FAF65583-B8F6-40EA-862C-E4025F5D5778}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FAF65583-B8F6-40EA-862C-E4025F5D5778}" name="Table114" displayName="Table114" ref="A1:E15" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
+  <autoFilter ref="A1:E15" xr:uid="{FAF65583-B8F6-40EA-862C-E4025F5D5778}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9DCDC563-2DFF-40C4-9194-5C07503E012F}" name="What we're doing" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{D5AE45F1-A084-45BD-B4F4-32098DA0FE85}" name="Code" dataDxfId="3"/>
@@ -6043,7 +6200,7 @@
         <v>274</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D7" s="24"/>
     </row>
@@ -6059,22 +6216,22 @@
     </row>
     <row r="9" spans="1:4" ht="105">
       <c r="A9" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" s="38" t="s">
         <v>317</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>319</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>318</v>
       </c>
       <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:4" ht="75">
       <c r="A10" s="38" t="s">
+        <v>323</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>324</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>325</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24" t="e" vm="14">
@@ -6091,10 +6248,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B3B599-2C6A-4CA8-B2F0-63091B448B87}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6193,11 +6350,11 @@
       <c r="A7" s="34" t="s">
         <v>294</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="41" t="s">
+        <v>329</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>299</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>300</v>
       </c>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
@@ -6226,40 +6383,83 @@
     </row>
     <row r="10" spans="1:5" ht="180">
       <c r="A10" s="39" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="D10" s="31"/>
+        <v>322</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>330</v>
+      </c>
       <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5" ht="165">
       <c r="A11" s="39" t="s">
+        <v>320</v>
+      </c>
+      <c r="B11" s="40" t="s">
         <v>321</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>322</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:5" ht="135">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="42" t="s">
+        <v>331</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>334</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31" t="e" vm="15">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="315">
+      <c r="A13" s="42" t="s">
+        <v>332</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+    </row>
+    <row r="14" spans="1:5" ht="105">
+      <c r="A14" s="42" t="s">
+        <v>337</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+    </row>
+    <row r="15" spans="1:5" ht="135">
+      <c r="A15" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="B15" s="40" t="s">
         <v>326</v>
       </c>
-      <c r="B12" s="40" t="s">
-        <v>327</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>329</v>
-      </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
+      <c r="C15" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6299,7 +6499,7 @@
     </row>
     <row r="2" spans="1:3" ht="90">
       <c r="A2" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>122</v>
@@ -6308,40 +6508,40 @@
     </row>
     <row r="3" spans="1:3" ht="75">
       <c r="A3" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>308</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="C3" s="36" t="s">
         <v>309</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="180">
       <c r="A4" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>311</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="120">
       <c r="A5" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>123</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="90">
       <c r="A6" s="36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>124</v>
@@ -6352,24 +6552,24 @@
     </row>
     <row r="7" spans="1:3" ht="180">
       <c r="A7" s="37" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B7" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>313</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="180">
       <c r="A8" s="37" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>125</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="165">

</xml_diff>

<commit_message>
Added small info to Python cheatsheet
</commit_message>
<xml_diff>
--- a/Python, NumPy, Pandas, MatPlotLib, Scikit-learn.xlsx
+++ b/Python, NumPy, Pandas, MatPlotLib, Scikit-learn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0029D93E-FB2A-4B5B-A083-0AF0E04A06F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D16EAF-A0F6-4DBC-A633-0334A38254A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="5895" windowWidth="29040" windowHeight="15720" tabRatio="685" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="685" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Python Intermediate" sheetId="7" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="379">
   <si>
     <t>What we're doing</t>
   </si>
@@ -4544,12 +4544,6 @@
 Note that h.history also contains other metrics like accuracy or validation loss if you have configured the model to record them during training.</t>
   </si>
   <si>
-    <t>plt.plot(normalised_x, y, c="b")
-plt.plot(x, y, c="r")
-plt.plot(x, model.predict(normalised_x), c="g")
-plt.show()</t>
-  </si>
-  <si>
     <r>
       <t>print(</t>
     </r>
@@ -5518,6 +5512,95 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> - Transposes the dataset (swaps the columns and rows with one another)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">plt.plot(normalised_x, y, c="b")
+plt.plot(x, y, c="r")
+plt.plot(x, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>model.predict(normalised_x),</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t xml:space="preserve"> c="g")
+plt.show()</t>
+    </r>
+  </si>
+  <si>
+    <t>K-Folding</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">K-folding is a way of creating and testing our models where we split our data into two sets: one set for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>training</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and one set for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>validation/testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. It's a technique used specifically for smaller data sets, so not for large models like ChatGPT/others</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
     </r>
   </si>
 </sst>
@@ -5525,12 +5608,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5749,6 +5839,12 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5837,95 +5933,95 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5934,52 +6030,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5988,23 +6087,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6960,8 +7059,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{46C16BA2-61C0-4599-920E-0C9F452559FA}" name="Table210" displayName="Table210" ref="A1:D10" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:D10" xr:uid="{46C16BA2-61C0-4599-920E-0C9F452559FA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{46C16BA2-61C0-4599-920E-0C9F452559FA}" name="Table210" displayName="Table210" ref="A1:D11" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:D11" xr:uid="{46C16BA2-61C0-4599-920E-0C9F452559FA}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{23F4172E-BA4C-4B53-8A90-E0059ED1DE4A}" name="Concepts" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{04ADC2BE-761C-4A23-BD42-73FBD7BB9ACC}" name="General Understanding" dataDxfId="14"/>
@@ -7694,10 +7793,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87179907-4FD1-4D78-B59B-9D41D9D2BE6B}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7826,6 +7925,16 @@
       <c r="D10" s="24" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
+    </row>
+    <row r="11" spans="1:4" ht="45">
+      <c r="A11" s="56" t="s">
+        <v>377</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>378</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8084,8 +8193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C63454-64FF-4807-AE72-E52F6B402F7B}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8161,7 +8270,7 @@
         <v>363</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>364</v>
@@ -8169,16 +8278,16 @@
     </row>
     <row r="6" spans="1:5" ht="150">
       <c r="A6" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>376</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>367</v>
       </c>
-      <c r="B6" s="44" t="s">
-        <v>365</v>
-      </c>
-      <c r="C6" s="50" t="s">
+      <c r="D6" s="50" t="s">
         <v>368</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -8701,7 +8810,7 @@
     </row>
     <row r="8" spans="1:3" ht="180">
       <c r="A8" s="53" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>180</v>
@@ -8712,10 +8821,10 @@
     </row>
     <row r="9" spans="1:3" ht="30">
       <c r="A9" s="53" t="s">
+        <v>370</v>
+      </c>
+      <c r="B9" s="53" t="s">
         <v>371</v>
-      </c>
-      <c r="B9" s="53" t="s">
-        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -8897,7 +9006,7 @@
         <v>53</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>54</v>
@@ -8923,7 +9032,7 @@
         <v>57</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>56</v>
@@ -9017,7 +9126,7 @@
         <v>229</v>
       </c>
       <c r="B13" s="54" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C13" s="54" t="s">
         <v>206</v>
@@ -9037,7 +9146,7 @@
         <v>231</v>
       </c>
       <c r="B15" s="54" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C15" s="22"/>
     </row>
@@ -9052,7 +9161,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="75">
+    <row r="17" spans="1:3" ht="60">
       <c r="A17" s="48" t="s">
         <v>345</v>
       </c>
@@ -9076,7 +9185,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>